<commit_message>
Project "project-name" is saved Author: admin. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/Example 2 - Corporate Rating/Corporate Rating.xlsx
+++ b/DESIGN/rules/Example 2 - Corporate Rating/Corporate Rating.xlsx
@@ -4,23 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="285" windowWidth="14805" windowHeight="7830" tabRatio="860"/>
+    <workbookView tabRatio="860" windowHeight="7830" windowWidth="14805" xWindow="240" yWindow="285"/>
   </bookViews>
   <sheets>
-    <sheet name="Rating Algorithm" sheetId="4" r:id="rId1"/>
-    <sheet name="Algorithm Tests" sheetId="6" r:id="rId2"/>
-    <sheet name="Financial Rating" sheetId="7" r:id="rId3"/>
-    <sheet name="Risk of Profile" sheetId="8" r:id="rId4"/>
-    <sheet name="Risk of Profile Tests" sheetId="9" r:id="rId5"/>
-    <sheet name="Risk of Operations" sheetId="11" r:id="rId6"/>
-    <sheet name="Risk of Oper Tests" sheetId="12" r:id="rId7"/>
-    <sheet name="Risk of Geography" sheetId="13" r:id="rId8"/>
-    <sheet name="Risk Groups" sheetId="10" r:id="rId9"/>
-    <sheet name="Corporate Rating" sheetId="14" r:id="rId10"/>
-    <sheet name="Set NonZero Values" sheetId="3" r:id="rId11"/>
-    <sheet name="Domain" sheetId="1" r:id="rId12"/>
-    <sheet name="Vocabulary" sheetId="2" r:id="rId13"/>
-    <sheet name="Test Data" sheetId="5" r:id="rId14"/>
+    <sheet name="Rating Algorithm" r:id="rId1" sheetId="4"/>
+    <sheet name="Algorithm Tests" r:id="rId2" sheetId="6"/>
+    <sheet name="Financial Rating" r:id="rId3" sheetId="7"/>
+    <sheet name="Risk of Profile" r:id="rId4" sheetId="8"/>
+    <sheet name="Risk of Profile Tests" r:id="rId5" sheetId="9"/>
+    <sheet name="Risk of Operations" r:id="rId6" sheetId="11"/>
+    <sheet name="Risk of Oper Tests" r:id="rId7" sheetId="12"/>
+    <sheet name="Risk of Geography" r:id="rId8" sheetId="13"/>
+    <sheet name="Risk Groups" r:id="rId9" sheetId="10"/>
+    <sheet name="Corporate Rating" r:id="rId10" sheetId="14"/>
+    <sheet name="Set NonZero Values" r:id="rId11" sheetId="3"/>
+    <sheet name="Domain" r:id="rId12" sheetId="1"/>
+    <sheet name="Vocabulary" r:id="rId13" sheetId="2"/>
+    <sheet name="Test Data" r:id="rId14" sheetId="5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
@@ -3467,6 +3467,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3575,7 +3576,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <charset val="204"/>
@@ -3583,7 +3584,7 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3606,7 +3607,7 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3681,7 +3682,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3693,13 +3694,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0" tint="-0.34998626667073579" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
+        <fgColor theme="2" tint="-0.249977111117893" rgb="FBEEC9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3711,7 +3712,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="0" tint="-0.14999847407452621" rgb="FFFFFF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3885,397 +3886,397 @@
     </border>
   </borders>
   <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="24" numFmtId="0" xfId="2"/>
   </cellStyleXfs>
   <cellXfs count="156">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="7" fillId="4" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="10" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="7" fontId="11" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="4" fillId="0" fontId="12" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="7" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="7" fontId="3" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="4" fillId="0" fontId="15" numFmtId="0" xfId="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="4" fillId="0" fontId="18" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="21" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="21" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="21" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="21" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="6" fillId="0" fontId="21" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="6" fontId="19" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="6" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="6" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="14" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="6" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="6" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="10" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="10" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="7" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="4" fillId="0" fontId="15" numFmtId="0" xfId="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="17" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="7" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="0" fillId="0" fontId="22" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="23" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="6" fillId="7" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="7" fontId="14" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="10" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="10" fillId="7" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="7" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFill="1" borderId="12" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="0" fillId="3" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="14" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="14" fillId="7" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="13" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="23" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="8" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="17" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="17" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="22" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="6" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="15" fillId="6" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="6" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="15" fillId="6" fontId="3" numFmtId="16" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFont="1" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="16" fontId="3" fillId="6" borderId="9" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="9" fillId="6" fontId="3" numFmtId="16" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="15" fillId="6" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="7" fontId="14" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="11" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="24" numFmtId="0" quotePrefix="1" xfId="2"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="23" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="10" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="1" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyFont="1" borderId="4" fillId="0" fontId="18" numFmtId="0" quotePrefix="1" xfId="1"/>
+    <xf applyFont="1" borderId="4" fillId="0" fontId="12" numFmtId="0" quotePrefix="1" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="14" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="11" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="11" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="3" numFmtId="0" quotePrefix="1" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="13" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="13" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="23" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="3" fontId="25" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="6" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="7" fontId="14" numFmtId="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="23" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="0" fillId="5" fontId="17" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="6" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="2" fontId="19" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="2" fontId="19" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="2" fillId="0" fontId="13" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="5" fillId="2" fontId="13" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="17" name="Heading 2" xfId="1"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium9" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -4288,7 +4289,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
@@ -4328,14 +4329,14 @@
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst>
-            <a:gd name="adj" fmla="val 16667"/>
+            <a:gd fmla="val 16667" name="adj"/>
           </a:avLst>
         </a:prstGeom>
         <a:ln>
           <a:noFill/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw blurRad="50800" dist="38100" dir="2700000" algn="tl" rotWithShape="0">
+          <a:outerShdw algn="tl" blurRad="50800" dir="2700000" dist="38100" rotWithShape="0">
             <a:prstClr val="black">
               <a:alpha val="40000"/>
             </a:prstClr>
@@ -4343,12 +4344,12 @@
         </a:effectLst>
         <a:scene3d>
           <a:camera prst="orthographicFront"/>
-          <a:lightRig rig="contrasting" dir="t">
+          <a:lightRig dir="t" rig="contrasting">
             <a:rot lat="0" lon="0" rev="4200000"/>
           </a:lightRig>
         </a:scene3d>
         <a:sp3d prstMaterial="plastic">
-          <a:bevelT w="381000" h="114300" prst="relaxedInset"/>
+          <a:bevelT h="114300" prst="relaxedInset" w="381000"/>
           <a:contourClr>
             <a:srgbClr val="969696"/>
           </a:contourClr>
@@ -4365,10 +4366,10 @@
   <a:themeElements>
     <a:clrScheme name="Trek">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="4E3B30"/>
@@ -4550,19 +4551,19 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="10000" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="10000">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -4572,7 +4573,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="76200" dist="50800" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="76200" dir="5400000" dist="50800" rotWithShape="0">
               <a:srgbClr val="4E3B30">
                 <a:alpha val="60000"/>
               </a:srgbClr>
@@ -4581,7 +4582,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="76200" dist="50800" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="76200" dir="5400000" dist="50800" rotWithShape="0">
               <a:srgbClr val="4E3B30">
                 <a:alpha val="60000"/>
               </a:srgbClr>
@@ -4591,32 +4592,32 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="tl">
+            <a:lightRig dir="tl" rig="threePt">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d prstMaterial="metal">
-            <a:bevelT w="10000" h="10000"/>
+            <a:bevelT h="10000" w="10000"/>
           </a:sp3d>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="76200" dist="50800" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="76200" dir="5400000" dist="50800" rotWithShape="0">
               <a:srgbClr val="4E3B30">
                 <a:alpha val="60000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
           <a:scene3d>
-            <a:camera prst="obliqueTopLeft" fov="600000">
+            <a:camera fov="600000" prst="obliqueTopLeft">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="balanced" dir="t">
+            <a:lightRig dir="t" rig="balanced">
               <a:rot lat="0" lon="0" rev="19200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d contourW="12700" prstMaterial="matte">
-            <a:bevelT w="60000" h="50800"/>
+            <a:bevelT h="50800" w="60000"/>
             <a:contourClr>
               <a:schemeClr val="phClr">
                 <a:shade val="60000"/>
@@ -4643,7 +4644,7 @@
               </a:schemeClr>
             </a:duotone>
           </a:blip>
-          <a:tile tx="0" ty="0" sx="95000" sy="95000" flip="none" algn="t"/>
+          <a:tile algn="t" flip="none" sx="95000" sy="95000" tx="0" ty="0"/>
         </a:blipFill>
         <a:blipFill>
           <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
@@ -4671,29 +4672,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B3:I96"/>
+  <dimension ref="B3:J96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
-    <col min="5" max="5" width="40.88671875" customWidth="1"/>
-    <col min="6" max="6" width="56.21875" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="12.0" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="13.0" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="40.88671875" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="56.21875" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>61</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="2:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:8" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -4702,7 +4703,7 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="2:8" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="105" r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="C6" s="133" t="s">
         <v>475</v>
@@ -4720,7 +4721,7 @@
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
     </row>
-    <row r="8" spans="2:8" ht="19.5" x14ac:dyDescent="0.35">
+    <row ht="19.5" r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="12"/>
       <c r="C8" s="129" t="s">
         <v>423</v>
@@ -4730,7 +4731,7 @@
       <c r="F8" s="129"/>
       <c r="G8" s="12"/>
     </row>
-    <row r="9" spans="2:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="57.75" r="9" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="C9" s="57" t="s">
         <v>62</v>
@@ -4825,7 +4826,7 @@
       </c>
       <c r="G15" s="12"/>
     </row>
-    <row r="16" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15.75" r="16" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
       <c r="C16" s="132" t="s">
         <v>500</v>
@@ -4837,7 +4838,7 @@
       </c>
       <c r="G16" s="12"/>
     </row>
-    <row r="17" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="16.5" r="17" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B17" s="12"/>
       <c r="C17" s="132" t="s">
         <v>501</v>
@@ -4854,7 +4855,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="16.5" r="18" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="12"/>
       <c r="C18" s="126" t="s">
         <v>378</v>
@@ -4899,7 +4900,7 @@
       <c r="F21" s="12"/>
       <c r="G21" s="12"/>
     </row>
-    <row r="22" spans="2:8" ht="19.5" x14ac:dyDescent="0.35">
+    <row ht="19.5" r="22" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B22" s="12"/>
       <c r="C22" s="129" t="s">
         <v>424</v>
@@ -4912,7 +4913,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="23" spans="2:8" ht="115.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="115.5" r="23" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B23" s="12"/>
       <c r="C23" s="57" t="s">
         <v>62</v>
@@ -5150,7 +5151,7 @@
       </c>
       <c r="G39" s="12"/>
     </row>
-    <row r="40" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15.75" r="40" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B40" s="12"/>
       <c r="C40" s="127" t="s">
         <v>190</v>
@@ -5206,7 +5207,7 @@
       </c>
       <c r="G43" s="12"/>
     </row>
-    <row r="44" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15.75" r="44" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B44" s="12"/>
       <c r="C44" s="127" t="s">
         <v>197</v>
@@ -5220,7 +5221,7 @@
       </c>
       <c r="G44" s="12"/>
     </row>
-    <row r="45" spans="2:7" ht="28.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="28.5" r="45" spans="2:7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="12"/>
       <c r="C45" s="125" t="s">
         <v>200</v>
@@ -5234,7 +5235,7 @@
       </c>
       <c r="G45" s="12"/>
     </row>
-    <row r="46" spans="2:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="16.5" r="46" spans="2:7" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B46" s="12"/>
       <c r="C46" s="126" t="s">
         <v>203</v>
@@ -5264,7 +5265,7 @@
       <c r="F48" s="12"/>
       <c r="G48" s="12"/>
     </row>
-    <row r="49" spans="2:9" ht="19.5" x14ac:dyDescent="0.35">
+    <row ht="19.5" r="49" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B49" s="12"/>
       <c r="C49" s="129" t="s">
         <v>425</v>
@@ -5277,7 +5278,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="50" spans="2:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="48.75" r="50" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B50" s="12"/>
       <c r="C50" s="57" t="s">
         <v>62</v>
@@ -5319,7 +5320,7 @@
       </c>
       <c r="G52" s="12"/>
     </row>
-    <row r="53" spans="2:9" ht="27.75" x14ac:dyDescent="0.3">
+    <row ht="27.75" r="53" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B53" s="12"/>
       <c r="C53" s="125" t="s">
         <v>274</v>
@@ -5405,7 +5406,7 @@
       </c>
       <c r="G58" s="12"/>
     </row>
-    <row r="59" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15.75" r="59" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B59" s="12"/>
       <c r="C59" s="131" t="s">
         <v>293</v>
@@ -5419,7 +5420,7 @@
       </c>
       <c r="G59" s="12"/>
     </row>
-    <row r="60" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15.75" r="60" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B60" s="12"/>
       <c r="C60" s="125" t="s">
         <v>277</v>
@@ -5433,7 +5434,7 @@
       </c>
       <c r="G60" s="12"/>
     </row>
-    <row r="61" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="16.5" r="61" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B61" s="12"/>
       <c r="C61" s="127" t="s">
         <v>291</v>
@@ -5447,7 +5448,7 @@
       </c>
       <c r="G61" s="12"/>
     </row>
-    <row r="62" spans="2:9" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="42" r="62" spans="2:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B62" s="12"/>
       <c r="C62" s="125" t="s">
         <v>285</v>
@@ -5461,7 +5462,7 @@
       </c>
       <c r="G62" s="12"/>
     </row>
-    <row r="63" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="16.5" r="63" spans="2:9" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B63" s="12"/>
       <c r="C63" s="126" t="s">
         <v>498</v>
@@ -5503,7 +5504,7 @@
       <c r="F66" s="12"/>
       <c r="G66" s="12"/>
     </row>
-    <row r="67" spans="2:8" ht="19.5" x14ac:dyDescent="0.35">
+    <row ht="19.5" r="67" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B67" s="12"/>
       <c r="C67" s="129" t="s">
         <v>426</v>
@@ -5516,7 +5517,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="68" spans="2:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="60" r="68" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B68" s="12"/>
       <c r="C68" s="57" t="s">
         <v>62</v>
@@ -5670,7 +5671,7 @@
       </c>
       <c r="G78" s="12"/>
     </row>
-    <row r="79" spans="2:8" ht="55.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="55.5" r="79" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B79" s="12"/>
       <c r="C79" s="125" t="s">
         <v>285</v>
@@ -5684,7 +5685,7 @@
       </c>
       <c r="G79" s="12"/>
     </row>
-    <row r="80" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="16.5" r="80" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B80" s="12"/>
       <c r="C80" s="126" t="s">
         <v>499</v>
@@ -5726,7 +5727,7 @@
       <c r="F83" s="12"/>
       <c r="G83" s="12"/>
     </row>
-    <row r="84" spans="2:8" ht="19.5" x14ac:dyDescent="0.35">
+    <row ht="19.5" r="84" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B84" s="12"/>
       <c r="C84" s="129" t="s">
         <v>427</v>
@@ -5739,7 +5740,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="85" spans="2:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="61.5" r="85" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B85" s="12"/>
       <c r="C85" s="57" t="s">
         <v>62</v>
@@ -5795,7 +5796,7 @@
       </c>
       <c r="G88" s="12"/>
     </row>
-    <row r="89" spans="2:8" ht="27.75" x14ac:dyDescent="0.3">
+    <row ht="27.75" r="89" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B89" s="12"/>
       <c r="C89" s="123" t="s">
         <v>357</v>
@@ -5851,7 +5852,7 @@
       </c>
       <c r="G92" s="12"/>
     </row>
-    <row r="93" spans="2:8" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="42" r="93" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B93" s="12"/>
       <c r="C93" s="125" t="s">
         <v>285</v>
@@ -5865,7 +5866,7 @@
       </c>
       <c r="G93" s="12"/>
     </row>
-    <row r="94" spans="2:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row ht="16.5" r="94" spans="2:8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B94" s="12"/>
       <c r="C94" s="126" t="s">
         <v>500</v>
@@ -5985,33 +5986,33 @@
     <mergeCell ref="C39:D39"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H11" location="'Set NonZero Values'!A1" display="'Set NonZero Values'!A1"/>
-    <hyperlink ref="H17" location="'Risk Groups'!A1" display="'Risk Groups'!A1"/>
-    <hyperlink ref="H18" location="'Corporate Rating'!A1" display="'Corporate Rating'!A1"/>
-    <hyperlink ref="H22" location="'Financial Rating'!A1" display="'Financial Rating'!A1"/>
-    <hyperlink ref="H49" location="'Risk of Profile'!A1" display="'Risk of Profile'!A1"/>
-    <hyperlink ref="H67" location="'Risk of Operations'!A1" display="'Risk of Operations'!A1"/>
-    <hyperlink ref="H84" location="'Risk of Geography'!A1" display="'Risk of Geography'!A1"/>
+    <hyperlink display="'Set NonZero Values'!A1" location="'Set NonZero Values'!A1" ref="H11"/>
+    <hyperlink display="'Risk Groups'!A1" location="'Risk Groups'!A1" ref="H17"/>
+    <hyperlink display="'Corporate Rating'!A1" location="'Corporate Rating'!A1" ref="H18"/>
+    <hyperlink display="'Financial Rating'!A1" location="'Financial Rating'!A1" ref="H22"/>
+    <hyperlink display="'Risk of Profile'!A1" location="'Risk of Profile'!A1" ref="H49"/>
+    <hyperlink display="'Risk of Operations'!A1" location="'Risk of Operations'!A1" ref="H67"/>
+    <hyperlink display="'Risk of Geography'!A1" location="'Risk of Geography'!A1" ref="H84"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:G24"/>
+  <dimension ref="B1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="20.77734375" customWidth="1"/>
-    <col min="5" max="5" width="57.88671875" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="20.77734375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="57.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.3">
@@ -6019,20 +6020,20 @@
         <v>385</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:7" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>61</v>
       </c>
       <c r="C3" s="49"/>
     </row>
-    <row r="4" spans="2:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:7" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="2:7" ht="39.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="39.75" r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C6" s="12"/>
       <c r="D6" s="141" t="s">
         <v>478</v>
@@ -6046,7 +6047,7 @@
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
     </row>
-    <row r="8" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="8" spans="2:7" x14ac:dyDescent="0.3">
       <c r="C8" s="12"/>
       <c r="D8" s="135" t="s">
         <v>508</v>
@@ -6132,7 +6133,7 @@
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
     </row>
-    <row r="18" spans="3:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="18" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C18" s="12"/>
       <c r="D18" s="135" t="s">
         <v>373</v>
@@ -6150,7 +6151,7 @@
       </c>
       <c r="F19" s="12"/>
     </row>
-    <row r="20" spans="3:6" ht="41.25" x14ac:dyDescent="0.3">
+    <row ht="41.25" r="20" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C20" s="12"/>
       <c r="D20" s="76">
         <v>1</v>
@@ -6160,7 +6161,7 @@
       </c>
       <c r="F20" s="12"/>
     </row>
-    <row r="21" spans="3:6" ht="27.75" x14ac:dyDescent="0.3">
+    <row ht="27.75" r="21" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C21" s="12"/>
       <c r="D21" s="113">
         <v>2</v>
@@ -6170,7 +6171,7 @@
       </c>
       <c r="F21" s="12"/>
     </row>
-    <row r="22" spans="3:6" ht="41.25" x14ac:dyDescent="0.3">
+    <row ht="41.25" r="22" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C22" s="12"/>
       <c r="D22" s="113">
         <v>3</v>
@@ -6180,7 +6181,7 @@
       </c>
       <c r="F22" s="12"/>
     </row>
-    <row r="23" spans="3:6" ht="27.75" x14ac:dyDescent="0.3">
+    <row ht="27.75" r="23" spans="3:6" x14ac:dyDescent="0.3">
       <c r="C23" s="12"/>
       <c r="D23" s="112">
         <v>4</v>
@@ -6203,28 +6204,28 @@
     <mergeCell ref="D6:E6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G1" location="'Rating Algorithm'!A17" display="Rating Algorithm'!A17"/>
+    <hyperlink display="Rating Algorithm'!A17" location="'Rating Algorithm'!A17" ref="G1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.14999847407452621"/>
   </sheetPr>
-  <dimension ref="B1:H18"/>
+  <dimension ref="B1:I18"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.21875" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" customWidth="1"/>
-    <col min="5" max="5" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="12.109375" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="24.21875" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="20.5546875" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.109375" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="25.0" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
@@ -6232,13 +6233,13 @@
         <v>381</v>
       </c>
     </row>
-    <row r="3" spans="2:8" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:8" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>71</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="2:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:8" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -6247,7 +6248,7 @@
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
     </row>
-    <row r="6" spans="2:8" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="6" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="C6" s="129" t="s">
         <v>422</v>
@@ -6422,37 +6423,37 @@
     <mergeCell ref="C6:F6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H1" location="'Rating Algorithm'!A10" display="'Rating Algorithm'!A10"/>
+    <hyperlink display="'Rating Algorithm'!A10" location="'Rating Algorithm'!A10" ref="H1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="B3:G51"/>
+  <dimension ref="B3:H51"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="1"/>
+    <col min="1" max="2" style="1" width="8.88671875" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="12.6640625" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="32.33203125" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" style="1" width="20.5546875" collapsed="false"/>
+    <col min="6" max="16384" style="1" width="8.88671875" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="2:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:6" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -6460,7 +6461,7 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="17"/>
       <c r="C6" s="149" t="s">
         <v>31</v>
@@ -6566,7 +6567,7 @@
       <c r="E15" s="17"/>
       <c r="F15" s="17"/>
     </row>
-    <row r="16" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="16" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B16" s="17"/>
       <c r="C16" s="129" t="s">
         <v>32</v>
@@ -6722,7 +6723,7 @@
       <c r="E28" s="17"/>
       <c r="F28" s="17"/>
     </row>
-    <row r="29" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="29" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B29" s="17"/>
       <c r="C29" s="129" t="s">
         <v>33</v>
@@ -7021,34 +7022,34 @@
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C29:E29"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="2" tint="-9.9978637043366805E-2"/>
   </sheetPr>
-  <dimension ref="B3:E48"/>
+  <dimension ref="B3:F48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.44140625" customWidth="1"/>
-    <col min="2" max="2" width="6" customWidth="1"/>
-    <col min="3" max="3" width="24.109375" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.44140625" collapsed="false"/>
+    <col min="2" max="2" customWidth="true" width="6.0" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="21" width="24.109375" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:4" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="22"/>
     </row>
-    <row r="4" spans="2:4" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:4" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:4" x14ac:dyDescent="0.3">
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -7340,30 +7341,30 @@
       <c r="D48" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="B3:I53"/>
+  <dimension ref="B3:J53"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="15.109375" customWidth="1"/>
-    <col min="5" max="5" width="39.33203125" customWidth="1"/>
-    <col min="6" max="6" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.21875" customWidth="1"/>
-    <col min="9" max="9" width="45.6640625" customWidth="1"/>
+    <col min="4" max="4" customWidth="true" width="15.109375" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="39.33203125" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.6640625" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="12.21875" collapsed="false"/>
+    <col min="9" max="9" customWidth="true" width="45.6640625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:9" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="122" t="s">
         <v>485</v>
       </c>
@@ -7372,7 +7373,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:9" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="17"/>
       <c r="C5" s="17"/>
@@ -7381,7 +7382,7 @@
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
     </row>
-    <row r="6" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="17"/>
       <c r="C6" s="154" t="s">
         <v>105</v>
@@ -7511,7 +7512,7 @@
       <c r="F15" s="28"/>
       <c r="G15" s="28"/>
     </row>
-    <row r="16" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="149" t="s">
@@ -7689,7 +7690,7 @@
       <c r="F29" s="28"/>
       <c r="G29" s="28"/>
     </row>
-    <row r="30" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="30" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="152" t="s">
@@ -7947,7 +7948,7 @@
       <c r="F50" s="39"/>
       <c r="G50" s="28"/>
     </row>
-    <row r="51" spans="2:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="15.75" r="51" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B51" s="17"/>
       <c r="C51" s="17"/>
       <c r="D51" s="30" t="s">
@@ -7985,35 +7986,35 @@
     <mergeCell ref="D30:F30"/>
     <mergeCell ref="C6:F6"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="B3:F39"/>
+  <dimension ref="B3:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" customWidth="1"/>
-    <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="4" width="34.77734375" customWidth="1"/>
-    <col min="5" max="5" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="11.5546875" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="21.5546875" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="34.77734375" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="23.44140625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>109</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="2:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:6" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -8353,25 +8354,25 @@
     <mergeCell ref="C27:D27"/>
     <mergeCell ref="C34:D34"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="5" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="B1:G80"/>
+  <dimension ref="B1:H80"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.6640625" style="50" customWidth="1"/>
-    <col min="4" max="4" width="27.44140625" style="50" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" style="50" width="23.6640625" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="50" width="27.44140625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="27.44140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.3">
@@ -8379,13 +8380,13 @@
         <v>387</v>
       </c>
     </row>
-    <row r="3" spans="2:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:7" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>211</v>
       </c>
       <c r="C3" s="49"/>
     </row>
-    <row r="4" spans="2:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:7" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -8393,7 +8394,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="2:7" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="63.75" r="6" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="C6" s="141" t="s">
         <v>477</v>
@@ -8416,7 +8417,7 @@
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
     </row>
-    <row r="9" spans="2:7" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="9" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="C9" s="135" t="s">
         <v>479</v>
@@ -8452,8 +8453,8 @@
       <c r="C12" s="46" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="53">
-        <v>2</v>
+      <c r="D12" s="53" t="n">
+        <v>18.0</v>
       </c>
       <c r="E12" s="12"/>
       <c r="F12" s="12"/>
@@ -8494,7 +8495,7 @@
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
     </row>
-    <row r="17" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="17" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B17" s="12"/>
       <c r="C17" s="135" t="s">
         <v>480</v>
@@ -8572,7 +8573,7 @@
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
     </row>
-    <row r="25" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="25" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B25" s="12"/>
       <c r="C25" s="135" t="s">
         <v>481</v>
@@ -8650,7 +8651,7 @@
       <c r="E32" s="12"/>
       <c r="F32" s="12"/>
     </row>
-    <row r="33" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="33" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
       <c r="C33" s="155" t="s">
         <v>503</v>
@@ -8914,7 +8915,7 @@
       <c r="E56" s="12"/>
       <c r="F56" s="12"/>
     </row>
-    <row r="57" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="57" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B57" s="12"/>
       <c r="C57" s="135" t="s">
         <v>482</v>
@@ -8992,7 +8993,7 @@
       <c r="E64" s="12"/>
       <c r="F64" s="12"/>
     </row>
-    <row r="65" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="65" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B65" s="12"/>
       <c r="C65" s="135" t="s">
         <v>182</v>
@@ -9081,7 +9082,7 @@
       <c r="E73" s="12"/>
       <c r="F73" s="12"/>
     </row>
-    <row r="74" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="74" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B74" s="12"/>
       <c r="C74" s="135" t="s">
         <v>483</v>
@@ -9169,27 +9170,27 @@
     <mergeCell ref="C33:E33"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G1" location="'Rating Algorithm'!A21" display="'Rating Algorithm'!A21"/>
+    <hyperlink display="'Rating Algorithm'!A21" location="'Rating Algorithm'!A21" ref="G1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B1:K55"/>
+  <dimension ref="B1:L55"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
-    <col min="4" max="4" width="22.109375" customWidth="1"/>
-    <col min="5" max="5" width="25" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="25.5546875" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="22.109375" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="25.0" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" x14ac:dyDescent="0.3">
@@ -9197,7 +9198,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="3" spans="2:11" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:11" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>226</v>
       </c>
@@ -9205,7 +9206,7 @@
       <c r="D3" s="50"/>
       <c r="E3" s="50"/>
     </row>
-    <row r="4" spans="2:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="4" spans="2:11" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B4" s="50"/>
       <c r="C4" s="50"/>
       <c r="D4" s="50"/>
@@ -9222,7 +9223,7 @@
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
     </row>
-    <row r="6" spans="2:11" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="46.5" r="6" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="C6" s="141" t="s">
         <v>471</v>
@@ -9246,7 +9247,7 @@
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
     </row>
-    <row r="8" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="8" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
       <c r="C8" s="135" t="s">
         <v>228</v>
@@ -9350,7 +9351,7 @@
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
     </row>
-    <row r="16" spans="2:11" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="16" spans="2:11" x14ac:dyDescent="0.3">
       <c r="B16" s="12"/>
       <c r="C16" s="135" t="s">
         <v>484</v>
@@ -9503,7 +9504,7 @@
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
     </row>
-    <row r="27" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" s="12"/>
       <c r="C27" s="135" t="s">
         <v>251</v>
@@ -9583,7 +9584,7 @@
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
     </row>
-    <row r="33" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" s="12"/>
       <c r="C33" s="135" t="s">
         <v>248</v>
@@ -9596,7 +9597,7 @@
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
     </row>
-    <row r="34" spans="2:10" ht="27.75" x14ac:dyDescent="0.3">
+    <row ht="27.75" r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" s="12"/>
       <c r="C34" s="83" t="s">
         <v>250</v>
@@ -9678,7 +9679,7 @@
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
     </row>
-    <row r="40" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40" s="12"/>
       <c r="C40" s="135" t="s">
         <v>294</v>
@@ -9873,7 +9874,7 @@
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
     </row>
-    <row r="51" spans="2:10" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" s="12"/>
       <c r="C51" s="135" t="s">
         <v>269</v>
@@ -9960,35 +9961,35 @@
     <mergeCell ref="D10:D12"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="K1" location="'Rating Algorithm'!A48" display="'Rating Algorithm'!A48"/>
+    <hyperlink display="'Rating Algorithm'!A48" location="'Rating Algorithm'!A48" ref="K1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="B3:G21"/>
+  <dimension ref="B3:H21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.77734375" style="79" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" style="79" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="18.21875" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="79" width="21.77734375" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="79" width="17.5546875" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:7" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>243</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="2:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:7" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -10204,25 +10205,25 @@
     <mergeCell ref="C6:F6"/>
     <mergeCell ref="C16:D16"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B1:O48"/>
+  <dimension ref="B1:P48"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="29.5546875" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" customWidth="1"/>
-    <col min="8" max="8" width="7.44140625" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="29.5546875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.6640625" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="6.5546875" collapsed="false"/>
+    <col min="8" max="8" customWidth="true" width="7.44140625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:15" x14ac:dyDescent="0.3">
@@ -10230,13 +10231,13 @@
         <v>391</v>
       </c>
     </row>
-    <row r="3" spans="2:15" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>307</v>
       </c>
       <c r="C3" s="49"/>
     </row>
-    <row r="4" spans="2:15" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:15" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -10252,7 +10253,7 @@
       <c r="M5" s="12"/>
       <c r="N5" s="12"/>
     </row>
-    <row r="6" spans="2:15" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="39" r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="C6" s="141" t="s">
         <v>472</v>
@@ -10284,7 +10285,7 @@
       <c r="M7" s="12"/>
       <c r="N7" s="12"/>
     </row>
-    <row r="8" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
       <c r="C8" s="135" t="s">
         <v>308</v>
@@ -10388,7 +10389,7 @@
       <c r="M13" s="12"/>
       <c r="N13" s="12"/>
     </row>
-    <row r="14" spans="2:15" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
       <c r="C14" s="135" t="s">
         <v>313</v>
@@ -10511,7 +10512,7 @@
       <c r="M20" s="12"/>
       <c r="N20" s="12"/>
     </row>
-    <row r="21" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="21" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B21" s="12"/>
       <c r="C21" s="135" t="s">
         <v>314</v>
@@ -10528,7 +10529,7 @@
       <c r="M21" s="12"/>
       <c r="N21" s="12"/>
     </row>
-    <row r="22" spans="2:14" ht="27.75" x14ac:dyDescent="0.3">
+    <row ht="27.75" r="22" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B22" s="12"/>
       <c r="C22" s="83" t="s">
         <v>315</v>
@@ -10634,7 +10635,7 @@
       <c r="M27" s="12"/>
       <c r="N27" s="12"/>
     </row>
-    <row r="28" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="28" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B28" s="12"/>
       <c r="C28" s="135" t="s">
         <v>318</v>
@@ -10989,7 +10990,7 @@
       <c r="M42" s="12"/>
       <c r="N42" s="12"/>
     </row>
-    <row r="43" spans="2:14" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="43" spans="2:14" x14ac:dyDescent="0.3">
       <c r="B43" s="12"/>
       <c r="C43" s="135" t="s">
         <v>325</v>
@@ -11108,34 +11109,34 @@
     <mergeCell ref="C28:M28"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="O1" location="'Rating Algorithm'!A66" display="'Rating Algorithm'!A66"/>
+    <hyperlink display="'Rating Algorithm'!A66" location="'Rating Algorithm'!A66" ref="O1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0"/>
   </sheetPr>
-  <dimension ref="B3:E19"/>
+  <dimension ref="B3:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="34.33203125" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.6640625" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="121" t="s">
         <v>316</v>
       </c>
       <c r="C3" s="13"/>
     </row>
-    <row r="4" spans="2:5" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:5" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -11269,23 +11270,23 @@
     <mergeCell ref="C6:D6"/>
     <mergeCell ref="C14:D14"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B1:F24"/>
+  <dimension ref="B1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="39.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="39.88671875" collapsed="false"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="30.109375" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" x14ac:dyDescent="0.3">
@@ -11293,20 +11294,20 @@
         <v>393</v>
       </c>
     </row>
-    <row r="3" spans="2:6" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:6" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>345</v>
       </c>
       <c r="C3" s="49"/>
     </row>
-    <row r="4" spans="2:6" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:6" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
       <c r="E5" s="12"/>
     </row>
-    <row r="6" spans="2:6" ht="42" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="42" r="6" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B6" s="12"/>
       <c r="C6" s="141" t="s">
         <v>473</v>
@@ -11320,7 +11321,7 @@
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
     </row>
-    <row r="8" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="8" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B8" s="12"/>
       <c r="C8" s="135" t="s">
         <v>346</v>
@@ -11370,7 +11371,7 @@
       <c r="D13" s="12"/>
       <c r="E13" s="12"/>
     </row>
-    <row r="14" spans="2:6" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="14" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B14" s="12"/>
       <c r="C14" s="135" t="s">
         <v>349</v>
@@ -11420,7 +11421,7 @@
       <c r="D19" s="12"/>
       <c r="E19" s="12"/>
     </row>
-    <row r="20" spans="2:5" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B20" s="12"/>
       <c r="C20" s="135" t="s">
         <v>352</v>
@@ -11472,28 +11473,28 @@
     <mergeCell ref="C6:D6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="F1" location="'Rating Algorithm'!A83" display="'Rating Algorithm'!A83"/>
+    <hyperlink display="'Rating Algorithm'!A83" location="'Rating Algorithm'!A83" ref="F1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="0" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="B1:I44"/>
+  <dimension ref="B1:J44"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="12.44140625" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" width="16.21875" collapsed="false"/>
+    <col min="5" max="5" customWidth="true" width="18.0" collapsed="false"/>
+    <col min="6" max="6" customWidth="true" width="17.109375" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" width="10.6640625" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.3">
@@ -11501,13 +11502,13 @@
         <v>383</v>
       </c>
     </row>
-    <row r="3" spans="2:9" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
+    <row ht="21.75" r="3" spans="2:9" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="27" t="s">
         <v>296</v>
       </c>
       <c r="C3" s="49"/>
     </row>
-    <row r="4" spans="2:9" ht="16.5" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row ht="16.5" r="4" spans="2:9" thickTop="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C5" s="12"/>
       <c r="D5" s="12"/>
@@ -11516,7 +11517,7 @@
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
     </row>
-    <row r="6" spans="2:9" ht="124.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row customHeight="1" ht="124.5" r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C6" s="12"/>
       <c r="D6" s="141" t="s">
         <v>474</v>
@@ -11534,7 +11535,7 @@
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
     </row>
-    <row r="8" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C8" s="12"/>
       <c r="D8" s="135" t="s">
         <v>505</v>
@@ -11608,7 +11609,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="12"/>
     </row>
-    <row r="15" spans="2:9" ht="16.5" x14ac:dyDescent="0.3">
+    <row ht="16.5" r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="C15" s="12"/>
       <c r="D15" s="135" t="s">
         <v>506</v>
@@ -12081,8 +12082,8 @@
     <mergeCell ref="D6:G6"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="I1" location="'Rating Algorithm'!A16" display="'Rating Algorithm'!A16"/>
+    <hyperlink display="'Rating Algorithm'!A16" location="'Rating Algorithm'!A16" ref="I1"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>